<commit_message>
emploayee page excel operation
</commit_message>
<xml_diff>
--- a/src/test/java/com/jala/qa/DataLayer/EmployeeData.xlsx
+++ b/src/test/java/com/jala/qa/DataLayer/EmployeeData.xlsx
@@ -8,6 +8,8 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="44">
   <si>
     <t>First Name</t>
   </si>
@@ -136,13 +138,28 @@
   </si>
   <si>
     <t>Skills</t>
+  </si>
+  <si>
+    <t>AWS</t>
+  </si>
+  <si>
+    <t>DevOps</t>
+  </si>
+  <si>
+    <t>QA-Automation</t>
+  </si>
+  <si>
+    <t>WebServices</t>
+  </si>
+  <si>
+    <t>Middleware</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,6 +199,12 @@
       <color rgb="FF1F1F1F"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -226,7 +249,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -235,6 +258,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -516,10 +540,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -590,9 +615,11 @@
         <v>31</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="J2" s="4"/>
+        <v>35</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="3" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
@@ -622,7 +649,9 @@
       <c r="I3" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="J3" s="4"/>
+      <c r="J3" s="4" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="4" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
@@ -652,7 +681,9 @@
       <c r="I4" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="J4" s="4"/>
+      <c r="J4" s="8" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="5" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
@@ -682,7 +713,9 @@
       <c r="I5" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="4"/>
+      <c r="J5" s="8" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="6" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
@@ -712,7 +745,152 @@
       <c r="I6" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="J6" s="4"/>
+      <c r="J6" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="C6" r:id="rId5"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="14.453125" customWidth="1"/>
+    <col min="5" max="5" width="14.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="4">
+        <v>7865433453</v>
+      </c>
+      <c r="E2" s="6">
+        <v>45746</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="4">
+        <v>8765432890</v>
+      </c>
+      <c r="E3" s="6">
+        <v>36944</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="4">
+        <v>9876546345</v>
+      </c>
+      <c r="E4" s="6">
+        <v>37439</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="4">
+        <v>9865347867</v>
+      </c>
+      <c r="E5" s="6">
+        <v>44412</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="4">
+        <v>8765493837</v>
+      </c>
+      <c r="E6" s="6">
+        <v>36775</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>